<commit_message>
improvements (match finds the best fitness value for regression)
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>x0</t>
   </si>
@@ -25,7 +25,10 @@
     <t>f'</t>
   </si>
   <si>
-    <t>(f-f')^2</t>
+    <t>(f-f')^2 normalized</t>
+  </si>
+  <si>
+    <t>(f-f')^2 classic</t>
   </si>
 </sst>
 </file>
@@ -383,13 +386,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -402,141 +405,428 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>13</v>
+        <v>83521</v>
       </c>
       <c r="C2">
-        <v>14</v>
+        <v>87158</v>
       </c>
       <c r="D2">
-        <v>13.5</v>
+        <v>87157.99597575798</v>
       </c>
       <c r="E2">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>2.655876616128772E-14</v>
+      </c>
+      <c r="F2">
+        <v>1.619452385035841E-05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>13</v>
+        <v>81632</v>
       </c>
       <c r="C3">
-        <v>13</v>
+        <v>74287</v>
       </c>
       <c r="D3">
-        <v>13.5</v>
+        <v>74286.99524180366</v>
       </c>
       <c r="E3">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>3.712995541860694E-14</v>
+      </c>
+      <c r="F3">
+        <v>2.264043245264865E-05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>12</v>
+        <v>82277</v>
       </c>
       <c r="C4">
-        <v>12</v>
+        <v>62375</v>
       </c>
       <c r="D4">
-        <v>12.00000000000136</v>
+        <v>62374.96224954988</v>
       </c>
       <c r="E4">
-        <v>1.861156378244312E-24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>2.337135969570663E-12</v>
+      </c>
+      <c r="F4">
+        <v>0.001425096483938641</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>11</v>
+        <v>78349</v>
       </c>
       <c r="C5">
-        <v>11</v>
+        <v>63904</v>
       </c>
       <c r="D5">
-        <v>10.99999999999523</v>
+        <v>63904.00627640509</v>
       </c>
       <c r="E5">
-        <v>2.279916563349283E-23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>6.46043323492143E-14</v>
+      </c>
+      <c r="F5">
+        <v>3.939326084136255E-05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>78216</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>61954</v>
       </c>
       <c r="D6">
-        <v>10.00000000000838</v>
+        <v>61954.00531282049</v>
       </c>
       <c r="E6">
-        <v>7.029823516350316E-23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>4.629029997574734E-14</v>
+      </c>
+      <c r="F6">
+        <v>2.822606154889799E-05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>9</v>
+        <v>63483</v>
       </c>
       <c r="C7">
-        <v>9</v>
+        <v>62836</v>
       </c>
       <c r="D7">
-        <v>8.999999999989356</v>
+        <v>62835.9974089648</v>
       </c>
       <c r="E7">
-        <v>1.132932497126126E-22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>1.1009975084499E-14</v>
+      </c>
+      <c r="F7">
+        <v>6.71346339643649E-06</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>8</v>
+        <v>52243</v>
       </c>
       <c r="C8">
-        <v>8</v>
+        <v>67016</v>
       </c>
       <c r="D8">
-        <v>8.00000000000585</v>
+        <v>67016.009753197</v>
       </c>
       <c r="E8">
-        <v>3.421715415287985E-23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>1.560032707885569E-13</v>
+      </c>
+      <c r="F8">
+        <v>9.512485162341112E-05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>53558</v>
       </c>
       <c r="C9">
-        <v>7</v>
+        <v>64482</v>
       </c>
       <c r="D9">
-        <v>6.999999999997753</v>
+        <v>64482.00568542173</v>
       </c>
       <c r="E9">
-        <v>5.049419768229174E-24</v>
+        <v>5.301088809124646E-14</v>
+      </c>
+      <c r="F9">
+        <v>3.232402019681284E-05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>54685</v>
+      </c>
+      <c r="C10">
+        <v>62172</v>
+      </c>
+      <c r="D10">
+        <v>62172.00532368233</v>
+      </c>
+      <c r="E10">
+        <v>4.647977059794016E-14</v>
+      </c>
+      <c r="F10">
+        <v>2.834159354668098E-05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>54507</v>
+      </c>
+      <c r="C11">
+        <v>49524</v>
+      </c>
+      <c r="D11">
+        <v>49523.99757949099</v>
+      </c>
+      <c r="E11">
+        <v>9.608445204132538E-15</v>
+      </c>
+      <c r="F11">
+        <v>5.858863860307554E-06</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>48757</v>
+      </c>
+      <c r="C12">
+        <v>48480</v>
+      </c>
+      <c r="D12">
+        <v>48480.00462402251</v>
+      </c>
+      <c r="E12">
+        <v>3.506546409980269E-14</v>
+      </c>
+      <c r="F12">
+        <v>2.138158419954067E-05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>44455</v>
+      </c>
+      <c r="C13">
+        <v>44876</v>
+      </c>
+      <c r="D13">
+        <v>44876.00417088519</v>
+      </c>
+      <c r="E13">
+        <v>2.852963272457853E-14</v>
+      </c>
+      <c r="F13">
+        <v>1.739628323384087E-05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>48869</v>
+      </c>
+      <c r="C14">
+        <v>31926</v>
+      </c>
+      <c r="D14">
+        <v>31926.00179487233</v>
+      </c>
+      <c r="E14">
+        <v>5.283319024730905E-15</v>
+      </c>
+      <c r="F14">
+        <v>3.221566677054374E-06</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>32235</v>
+      </c>
+      <c r="C15">
+        <v>42462</v>
+      </c>
+      <c r="D15">
+        <v>42461.99784561976</v>
+      </c>
+      <c r="E15">
+        <v>7.61174844261693E-15</v>
+      </c>
+      <c r="F15">
+        <v>4.641354232097346E-06</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>41006</v>
+      </c>
+      <c r="C16">
+        <v>21787</v>
+      </c>
+      <c r="D16">
+        <v>21787.00021050921</v>
+      </c>
+      <c r="E16">
+        <v>7.267447477178973E-17</v>
+      </c>
+      <c r="F16">
+        <v>4.431412590613688E-08</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>35150</v>
+      </c>
+      <c r="C17">
+        <v>20550</v>
+      </c>
+      <c r="D17">
+        <v>20550.01211102101</v>
+      </c>
+      <c r="E17">
+        <v>2.405477098076482E-13</v>
+      </c>
+      <c r="F17">
+        <v>0.0001466768300647205</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>29272</v>
+      </c>
+      <c r="C18">
+        <v>15917</v>
+      </c>
+      <c r="D18">
+        <v>15916.99429901746</v>
+      </c>
+      <c r="E18">
+        <v>5.330146328441325E-14</v>
+      </c>
+      <c r="F18">
+        <v>3.250120187494834E-05</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>28595</v>
+      </c>
+      <c r="C19">
+        <v>15775</v>
+      </c>
+      <c r="D19">
+        <v>15775.0037127686</v>
+      </c>
+      <c r="E19">
+        <v>2.260661180455557E-14</v>
+      </c>
+      <c r="F19">
+        <v>1.378465071130766E-05</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>15816</v>
+      </c>
+      <c r="C20">
+        <v>14717</v>
+      </c>
+      <c r="D20">
+        <v>14717.00456064919</v>
+      </c>
+      <c r="E20">
+        <v>3.411088959443608E-14</v>
+      </c>
+      <c r="F20">
+        <v>2.079952104576056E-05</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>13053</v>
+      </c>
+      <c r="C21">
+        <v>13947</v>
+      </c>
+      <c r="D21">
+        <v>13947.00721488086</v>
+      </c>
+      <c r="E21">
+        <v>8.536857640679696E-14</v>
+      </c>
+      <c r="F21">
+        <v>5.205450584251848E-05</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>14595</v>
+      </c>
+      <c r="C22">
+        <v>11970</v>
+      </c>
+      <c r="D22">
+        <v>11969.99879115759</v>
+      </c>
+      <c r="E22">
+        <v>2.396509134882938E-15</v>
+      </c>
+      <c r="F22">
+        <v>1.46129997673601E-06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>